<commit_message>
+ 增加 xsend(key, count:=1, lbtn:=false, title := "") 发送xfold快捷键,调用对应功能 + 优化Cmds定义 @xfold.ini。加载逻辑同Settings，优化加载读取 [Cmds]，未读取到再加载[Cmds-default] + 优化Hotstrings定义 @xfold.ini。加载逻辑同Settings，优化加载读取 [Hotstrings]，未读取到再加载[Hotstrings-default] + 增加QuickLook窗口激活功能 例： Tab@explorer => showQuickLook({Tab}) + 增加show(title) 激活显示标题中包含指定文本的窗口，有多个窗口匹配时显示最近打开的窗口 + 增加xstr(str) 转义相关保留字符, ",",";","@","(",")" + 增加xfold-cmd命令行功能，支持以下命令格式     * cmd:      g table     * cmd pipe: table>g     * function: g(table) + 整理 xfold-cmd 命令行参考 @xfold-cmd.csv + xfold-cmd打包命令行工具 xmd.exe @xfold-cmd.ahk * 更新打包应用的icon * 补充调整快捷键定义 @keys-leexioua.txt * 补充调整Cmds定义 @xfold.ini * Esc代替LButton快捷键，未知原因失效 - 已恢复
</commit_message>
<xml_diff>
--- a/xfold/xfold-shortcuts.xlsx
+++ b/xfold/xfold-shortcuts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Links\ahk\xfold\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F58AAD15-7141-4F52-A83A-03121D205948}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6C3E0DA-D10B-4857-9F71-F09752C3C412}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="20186" windowHeight="12920" xr2:uid="{73FB8399-4C17-4E0F-81A6-69D82FFF20BC}"/>
   </bookViews>
@@ -120,7 +120,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="235">
   <si>
     <t>LButton+单键</t>
   </si>
@@ -1659,10 +1659,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M45"/>
+  <dimension ref="A1:M50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.87890625" defaultRowHeight="12.7" x14ac:dyDescent="0.45"/>
@@ -1717,7 +1717,9 @@
       <c r="A2" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="2"/>
+      <c r="B2" s="2" t="s">
+        <v>162</v>
+      </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -1751,9 +1753,7 @@
       <c r="A4" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>162</v>
-      </c>
+      <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -2367,10 +2367,10 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A31" s="9" t="s">
-        <v>216</v>
+        <v>161</v>
       </c>
       <c r="B31" s="13" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="C31" s="12"/>
       <c r="D31" s="2"/>
@@ -2389,10 +2389,10 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A32" s="9" t="s">
-        <v>215</v>
-      </c>
-      <c r="B32" s="14" t="s">
-        <v>218</v>
+        <v>122</v>
+      </c>
+      <c r="B32" s="13" t="s">
+        <v>162</v>
       </c>
       <c r="C32" s="12"/>
       <c r="D32" s="2"/>
@@ -2415,10 +2415,10 @@
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A33" s="9" t="s">
-        <v>165</v>
+        <v>216</v>
       </c>
       <c r="B33" s="13" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="C33" s="12"/>
       <c r="D33" s="2"/>
@@ -2437,10 +2437,10 @@
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A34" s="9" t="s">
-        <v>130</v>
-      </c>
-      <c r="B34" s="13" t="s">
-        <v>77</v>
+        <v>215</v>
+      </c>
+      <c r="B34" s="14" t="s">
+        <v>218</v>
       </c>
       <c r="C34" s="12"/>
       <c r="D34" s="2"/>
@@ -2459,10 +2459,10 @@
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A35" s="9" t="s">
-        <v>131</v>
+        <v>165</v>
       </c>
       <c r="B35" s="13" t="s">
-        <v>76</v>
+        <v>164</v>
       </c>
       <c r="C35" s="12"/>
       <c r="D35" s="2"/>
@@ -2481,10 +2481,10 @@
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A36" s="9" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="B36" s="13" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C36" s="12"/>
       <c r="D36" s="2"/>
@@ -2498,8 +2498,12 @@
       <c r="M36" s="2"/>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A37" s="9"/>
-      <c r="B37" s="13"/>
+      <c r="A37" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="B37" s="13" t="s">
+        <v>76</v>
+      </c>
       <c r="C37" s="12"/>
       <c r="D37" s="2"/>
       <c r="F37" s="5"/>
@@ -2512,8 +2516,12 @@
       <c r="M37" s="2"/>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A38" s="9"/>
-      <c r="B38" s="13"/>
+      <c r="A38" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="B38" s="13" t="s">
+        <v>79</v>
+      </c>
       <c r="C38" s="12"/>
       <c r="D38" s="2"/>
       <c r="F38" s="5"/>
@@ -2622,6 +2630,76 @@
       <c r="K45" s="13"/>
       <c r="L45" s="11"/>
       <c r="M45" s="2"/>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A46" s="9"/>
+      <c r="B46" s="19"/>
+      <c r="C46" s="12"/>
+      <c r="D46" s="10"/>
+      <c r="F46" s="5"/>
+      <c r="G46" s="16"/>
+      <c r="H46" s="17"/>
+      <c r="I46" s="13"/>
+      <c r="J46" s="17"/>
+      <c r="K46" s="13"/>
+      <c r="L46" s="11"/>
+      <c r="M46" s="2"/>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A47" s="9"/>
+      <c r="B47" s="19"/>
+      <c r="C47" s="12"/>
+      <c r="D47" s="10"/>
+      <c r="F47" s="5"/>
+      <c r="G47" s="16"/>
+      <c r="H47" s="17"/>
+      <c r="I47" s="13"/>
+      <c r="J47" s="17"/>
+      <c r="K47" s="13"/>
+      <c r="L47" s="11"/>
+      <c r="M47" s="2"/>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A48" s="9"/>
+      <c r="B48" s="19"/>
+      <c r="C48" s="12"/>
+      <c r="D48" s="10"/>
+      <c r="F48" s="5"/>
+      <c r="G48" s="16"/>
+      <c r="H48" s="17"/>
+      <c r="I48" s="13"/>
+      <c r="J48" s="17"/>
+      <c r="K48" s="13"/>
+      <c r="L48" s="11"/>
+      <c r="M48" s="2"/>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A49" s="9"/>
+      <c r="B49" s="19"/>
+      <c r="C49" s="12"/>
+      <c r="D49" s="10"/>
+      <c r="F49" s="5"/>
+      <c r="G49" s="16"/>
+      <c r="H49" s="17"/>
+      <c r="I49" s="13"/>
+      <c r="J49" s="17"/>
+      <c r="K49" s="13"/>
+      <c r="L49" s="11"/>
+      <c r="M49" s="2"/>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A50" s="9"/>
+      <c r="B50" s="19"/>
+      <c r="C50" s="12"/>
+      <c r="D50" s="10"/>
+      <c r="F50" s="5"/>
+      <c r="G50" s="16"/>
+      <c r="H50" s="17"/>
+      <c r="I50" s="13"/>
+      <c r="J50" s="17"/>
+      <c r="K50" s="13"/>
+      <c r="L50" s="11"/>
+      <c r="M50" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -2649,8 +2727,8 @@
   </sheetPr>
   <dimension ref="A1:M50"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.87890625" defaultRowHeight="12.7" x14ac:dyDescent="0.45"/>

</xml_diff>